<commit_message>
QA 3, 4, 5
</commit_message>
<xml_diff>
--- a/Lab/Lab2_QA/QA.xlsx
+++ b/Lab/Lab2_QA/QA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SE_Group16\Lab\Lab2_QA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HocKy2\CNPM\SE_Group16\Lab\Lab2_QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA038F3-927F-4AC3-AD30-03B57643E6CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BB159A-C306-4925-81CB-5A5DB6BF0DD9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>No.</t>
   </si>
@@ -69,6 +69,34 @@
   </si>
   <si>
     <t>Theo như tài liệ SRS version 1.0.1 ở trang 62 có mô tả màn hình xóa một customer nhưng lại không có mô tả trường hợp bấm vào nút xóa thì có cần phải xác nhận lại việc xóa hay không. Theo tôi thì cần phải có một thông báo xác nhận lại việc xóa để tránh việc xóa nhầm một customer dẫn đến hậu quả không đáng có. Tôi hiểu như vậy có đúng không? Mong các bạn confirm.</t>
+  </si>
+  <si>
+    <t>SC01
+(Login)</t>
+  </si>
+  <si>
+    <t>Trong tài liệu SRS version 1.0.1 ở trang 51 có mô tả màn hình Login nhưng không có nút Nhớ mật khẩu.Theo tôi hiểu thì cần phải có thêm nút Nhớ mật khẩu có đúng không?</t>
+  </si>
+  <si>
+    <t>Bùi Thiên Hào</t>
+  </si>
+  <si>
+    <t>27/03/2021</t>
+  </si>
+  <si>
+    <t>SC02
+(List user in a division)</t>
+  </si>
+  <si>
+    <t>Trong tài liệu SRS version 1.0.1 ở trang 51 có mô tả màn hình List users chưa có Nút sắp xếp. Theo tôi muốn thêm Nút sắp xếp thì cần có phải thêm không?</t>
+  </si>
+  <si>
+    <t>SC04
+(View details user)</t>
+  </si>
+  <si>
+    <t>Trong tài liệu SRS version 1.0.1 ở trang 53 có mô tả màn hình View details user, màn hình có thể hiển thị tài khoản nào hoạt động thì để active, không hoạt động thì để off.
+Tôi nói như vậy có đúng không?</t>
   </si>
 </sst>
 </file>
@@ -97,7 +125,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,6 +141,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -144,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -167,6 +207,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -450,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D4:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,41 +591,71 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D7" s="5">
+    <row r="7" spans="4:11" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="D7" s="9">
         <v>3</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-    </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D8" s="5">
+      <c r="E7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="4:11" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="D8" s="12">
         <v>4</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-    </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D9" s="5">
+      <c r="E8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="4:11" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="D9" s="9">
         <v>5</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
+      <c r="E9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D10" s="5">

</xml_diff>

<commit_message>
QA 6, 7, 8, 9, 10
</commit_message>
<xml_diff>
--- a/Lab/Lab2_QA/QA.xlsx
+++ b/Lab/Lab2_QA/QA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HocKy2\CNPM\SE_Group16\Lab\Lab2_QA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NM_CNPM\SE_Group16\Lab\Lab2_QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BB159A-C306-4925-81CB-5A5DB6BF0DD9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22BA473-DE43-4C7A-B834-07C8E720F87C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>No.</t>
   </si>
@@ -97,17 +97,47 @@
   <si>
     <t>Trong tài liệu SRS version 1.0.1 ở trang 53 có mô tả màn hình View details user, màn hình có thể hiển thị tài khoản nào hoạt động thì để active, không hoạt động thì để off.
 Tôi nói như vậy có đúng không?</t>
+  </si>
+  <si>
+    <t>SC08: List Devisions</t>
+  </si>
+  <si>
+    <t>Trong tài liệu SRS version 1.0.1 trang 24 có mô tả màn hình hiển thị toàn bộ phòng ban/chi nhánh nhưng chưa có nút "Cập nhật "toàn bộ danh sách phòng ban/ chi nhánh. Theo tôi chúng ta cần có thêm nút "Cập nhật" nằm cạnh nút "Thêm mới" có đúng không ạ?</t>
+  </si>
+  <si>
+    <t>Trương Hoàng Vi</t>
+  </si>
+  <si>
+    <t>Trong tài liệu SRS version 1.0.1 trang 24 có mô tả màn hình hiển thị toàn bộ phòng ban/chi nhánh nhưng chưa có nút "Thu gọn- Mở rộng" danh sách hiển thị. Theo tôi chúng ta cần có thêm nút "Thu gọn- mở rộng" danh sách có đúng không ạ?</t>
+  </si>
+  <si>
+    <t>SC09: View detail divison</t>
+  </si>
+  <si>
+    <t>Trong tài liệu SRS version 1.0.1 trang 25 có nói đến việc cập nhật danh sách phòng ban/chi nhánh nhưng chưa cho phép xem lại lịch sử những lần cập nhật trước đó. Theo tôi , chúng ta cần có thêm nút "Xem lịch sử cập nhật" danh sách có đúng không ạ?</t>
+  </si>
+  <si>
+    <t>SC10: Add new division</t>
+  </si>
+  <si>
+    <t>Trong tài liệu SRS version 1.0.1, cuối trang 25,tại bước 4 của bảng Activities có nói đến việc Actor cần phải điều chỉnh sửa dữ liệu cho đúng nhưng không mô tả nếu nhập sai dữ liệu thì thông báo hiển thị như thế nào. Tôi đề xuấtphương án : Hiển thị dòng chữ màu đỏ "Dữ liệu nhập chưa phù hơp!!" ở ngay dưới chỗ nhập. Tôi hiểu như vậy có đúng không?</t>
+  </si>
+  <si>
+    <t>SC12: Delete Divison</t>
+  </si>
+  <si>
+    <t>rong tài liệu SRS version 1.0.1, cuối trang 26, đầu trang 27 có mô tả về việc xóa phòng ban/chi nhánh nhưng chưa có hiển thị khung thông báo đã xóa thành công, cũng như chưa cho phép hoàn tác lại thao tác sau khi thông báo xóa thành công. Theo tôi, cần xây dựng một khung có dòng chữ " Delete successfully" và nút hoàn tác( có đếm ngược thời gian )ở bên dưới dòng chữ đó. Tôi hiểu như vậy có đúng không ạ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -123,6 +153,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -157,7 +194,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -180,11 +217,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -225,6 +292,30 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -508,20 +599,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D4:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="56.21875" customWidth="1"/>
-    <col min="7" max="7" width="34.33203125" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="56.19921875" customWidth="1"/>
+    <col min="7" max="7" width="34.296875" customWidth="1"/>
+    <col min="8" max="8" width="14.59765625" customWidth="1"/>
+    <col min="10" max="10" width="15.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:11" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:11" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="2" t="s">
         <v>0</v>
       </c>
@@ -547,7 +638,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="4:11" ht="155.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:11" ht="155.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D5" s="5">
         <v>1</v>
       </c>
@@ -569,7 +660,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="4:11" ht="132" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:11" ht="132" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D6" s="5">
         <v>2</v>
       </c>
@@ -591,8 +682,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="4:11" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="D7" s="9">
+    <row r="7" spans="4:11" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="D7" s="5">
         <v>3</v>
       </c>
       <c r="E7" s="10" t="s">
@@ -613,8 +704,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="4:11" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="D8" s="12">
+    <row r="8" spans="4:11" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="D8" s="5">
         <v>4</v>
       </c>
       <c r="E8" s="13" t="s">
@@ -635,8 +726,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="4:11" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="D9" s="9">
+    <row r="9" spans="4:11" ht="55.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="5">
         <v>5</v>
       </c>
       <c r="E9" s="10" t="s">
@@ -657,65 +748,115 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:11" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="5">
         <v>6</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-    </row>
-    <row r="11" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="E10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="17">
+        <v>44282</v>
+      </c>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="4:11" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D11" s="5">
         <v>7</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-    </row>
-    <row r="12" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="E11" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="21">
+        <v>44282</v>
+      </c>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="4:11" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D12" s="5">
         <v>8</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-    </row>
-    <row r="13" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="E12" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="21">
+        <v>44282</v>
+      </c>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="4:11" ht="79.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" s="5">
         <v>9</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-    </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="E13" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="21">
+        <v>44283</v>
+      </c>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="4:11" ht="79.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="5">
         <v>10</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
+      <c r="E14" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="21">
+        <v>44283</v>
+      </c>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="19" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>